<commit_message>
Upload test data files
</commit_message>
<xml_diff>
--- a/t1_confection/A2_Structure_Lists.xlsx
+++ b/t1_confection/A2_Structure_Lists.xlsx
@@ -1396,64 +1396,64 @@
     <t>E6TRNOMOT</t>
   </si>
   <si>
+    <t>RESHID</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>CO2e_AFOLU</t>
+  </si>
+  <si>
     <t>CONTUR</t>
   </si>
   <si>
+    <t>turismo_residuos</t>
+  </si>
+  <si>
+    <t>CO2e_PIUP</t>
+  </si>
+  <si>
+    <t>CONVAR</t>
+  </si>
+  <si>
+    <t>CO2e_PP</t>
+  </si>
+  <si>
+    <t>CO2e_sources</t>
+  </si>
+  <si>
+    <t>FERT_ORG</t>
+  </si>
+  <si>
+    <t>DAPANI</t>
+  </si>
+  <si>
+    <t>CONHICK</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>contam_agua</t>
+  </si>
+  <si>
+    <t>CONHAB</t>
+  </si>
+  <si>
+    <t>CO2e_HFC</t>
+  </si>
+  <si>
+    <t>CO2e_TRN</t>
+  </si>
+  <si>
+    <t>CO2e_WASTE</t>
+  </si>
+  <si>
+    <t>CO2e_DE</t>
+  </si>
+  <si>
     <t>salud_residuos</t>
-  </si>
-  <si>
-    <t>contam_agua</t>
-  </si>
-  <si>
-    <t>RESHID</t>
-  </si>
-  <si>
-    <t>CO2e_HFC</t>
-  </si>
-  <si>
-    <t>CONHICK</t>
-  </si>
-  <si>
-    <t>DAPANI</t>
-  </si>
-  <si>
-    <t>FERT_ORG</t>
-  </si>
-  <si>
-    <t>CO2e_PIUP</t>
-  </si>
-  <si>
-    <t>CONVAR</t>
-  </si>
-  <si>
-    <t>CO2e_sources</t>
-  </si>
-  <si>
-    <t>CO2e_PP</t>
-  </si>
-  <si>
-    <t>Health</t>
-  </si>
-  <si>
-    <t>CO2e_DE</t>
-  </si>
-  <si>
-    <t>turismo_residuos</t>
-  </si>
-  <si>
-    <t>RM</t>
-  </si>
-  <si>
-    <t>CO2e_TRN</t>
-  </si>
-  <si>
-    <t>CONHAB</t>
-  </si>
-  <si>
-    <t>CO2e_AFOLU</t>
-  </si>
-  <si>
-    <t>CO2e_WASTE</t>
   </si>
   <si>
     <t>RD</t>

</xml_diff>

<commit_message>
Add the command line to run CPLEX with only one thread. Also, mek test with GLPK, CBC and CPLEX with only one thread. It is important to clarify the solver GLPK and CBC by default have one thread
</commit_message>
<xml_diff>
--- a/t1_confection/A2_Structure_Lists.xlsx
+++ b/t1_confection/A2_Structure_Lists.xlsx
@@ -1396,64 +1396,64 @@
     <t>E6TRNOMOT</t>
   </si>
   <si>
+    <t>FERT_ORG</t>
+  </si>
+  <si>
+    <t>DAPANI</t>
+  </si>
+  <si>
+    <t>CONVAR</t>
+  </si>
+  <si>
+    <t>CO2e_sources</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>CO2e_TRN</t>
+  </si>
+  <si>
+    <t>RESHID</t>
+  </si>
+  <si>
     <t>CO2e_PP</t>
   </si>
   <si>
+    <t>contam_agua</t>
+  </si>
+  <si>
+    <t>CO2e_AFOLU</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>CO2e_HFC</t>
+  </si>
+  <si>
     <t>CONTUR</t>
   </si>
   <si>
-    <t>FERT_ORG</t>
+    <t>CONHAB</t>
+  </si>
+  <si>
+    <t>CONHICK</t>
+  </si>
+  <si>
+    <t>turismo_residuos</t>
+  </si>
+  <si>
+    <t>salud_residuos</t>
+  </si>
+  <si>
+    <t>CO2e_WASTE</t>
+  </si>
+  <si>
+    <t>CO2e_DE</t>
   </si>
   <si>
     <t>CO2e_PIUP</t>
-  </si>
-  <si>
-    <t>turismo_residuos</t>
-  </si>
-  <si>
-    <t>CO2e_HFC</t>
-  </si>
-  <si>
-    <t>CO2e_AFOLU</t>
-  </si>
-  <si>
-    <t>CONHICK</t>
-  </si>
-  <si>
-    <t>CO2e_WASTE</t>
-  </si>
-  <si>
-    <t>Health</t>
-  </si>
-  <si>
-    <t>CONHAB</t>
-  </si>
-  <si>
-    <t>DAPANI</t>
-  </si>
-  <si>
-    <t>contam_agua</t>
-  </si>
-  <si>
-    <t>CO2e_DE</t>
-  </si>
-  <si>
-    <t>CO2e_TRN</t>
-  </si>
-  <si>
-    <t>CO2e_sources</t>
-  </si>
-  <si>
-    <t>RM</t>
-  </si>
-  <si>
-    <t>RESHID</t>
-  </si>
-  <si>
-    <t>CONVAR</t>
-  </si>
-  <si>
-    <t>salud_residuos</t>
   </si>
   <si>
     <t>RD</t>

</xml_diff>

<commit_message>
Add new module to create output files of Conversions parameters in A2 script
</commit_message>
<xml_diff>
--- a/t1_confection/A2_Structure_Lists.xlsx
+++ b/t1_confection/A2_Structure_Lists.xlsx
@@ -1396,28 +1396,55 @@
     <t>E6TRNOMOT</t>
   </si>
   <si>
+    <t>CO2e_HFC</t>
+  </si>
+  <si>
+    <t>contam_agua</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>CONHICK</t>
+  </si>
+  <si>
     <t>RESHID</t>
   </si>
   <si>
-    <t>RM</t>
+    <t>CO2e_TRN</t>
+  </si>
+  <si>
+    <t>CO2e_WASTE</t>
+  </si>
+  <si>
+    <t>turismo_residuos</t>
+  </si>
+  <si>
+    <t>DAPANI</t>
+  </si>
+  <si>
+    <t>CONHAB</t>
+  </si>
+  <si>
+    <t>CONTUR</t>
+  </si>
+  <si>
+    <t>CONVAR</t>
+  </si>
+  <si>
+    <t>CO2e_PIUP</t>
+  </si>
+  <si>
+    <t>CO2e_PP</t>
   </si>
   <si>
     <t>CO2e_AFOLU</t>
   </si>
   <si>
-    <t>CONTUR</t>
-  </si>
-  <si>
-    <t>turismo_residuos</t>
-  </si>
-  <si>
-    <t>CO2e_PIUP</t>
-  </si>
-  <si>
-    <t>CONVAR</t>
-  </si>
-  <si>
-    <t>CO2e_PP</t>
+    <t>salud_residuos</t>
   </si>
   <si>
     <t>CO2e_sources</t>
@@ -1426,34 +1453,7 @@
     <t>FERT_ORG</t>
   </si>
   <si>
-    <t>DAPANI</t>
-  </si>
-  <si>
-    <t>CONHICK</t>
-  </si>
-  <si>
-    <t>Health</t>
-  </si>
-  <si>
-    <t>contam_agua</t>
-  </si>
-  <si>
-    <t>CONHAB</t>
-  </si>
-  <si>
-    <t>CO2e_HFC</t>
-  </si>
-  <si>
-    <t>CO2e_TRN</t>
-  </si>
-  <si>
-    <t>CO2e_WASTE</t>
-  </si>
-  <si>
     <t>CO2e_DE</t>
-  </si>
-  <si>
-    <t>salud_residuos</t>
   </si>
   <si>
     <t>RD</t>

</xml_diff>